<commit_message>
refactor(translation): added language translations to locale
</commit_message>
<xml_diff>
--- a/utils/localisation_script/excel_to_json/hi/zlatest.xlsx
+++ b/utils/localisation_script/excel_to_json/hi/zlatest.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sreejithv/TW/projects/ekStep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/hi/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nireshkumarr/Documents/ekstep/crowdsource-dataplatform/utils/localisation_script/excel_to_json/hi/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6337E06C-C097-7046-BDEE-1AB3C60B8761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C48A93-8C61-F345-906C-B616A7E9EA77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="35840" windowHeight="21900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="35840" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="79">
   <si>
     <t>Error</t>
   </si>
@@ -103,19 +103,10 @@
     <t>हिंदी</t>
   </si>
   <si>
-    <t>Marathi</t>
-  </si>
-  <si>
     <t>मराठी</t>
   </si>
   <si>
-    <t>Tamil</t>
-  </si>
-  <si>
     <t>तमिल</t>
-  </si>
-  <si>
-    <t>Kannada</t>
   </si>
   <si>
     <t>कन्नड़</t>
@@ -127,31 +118,16 @@
     <t>मलयालम</t>
   </si>
   <si>
-    <t>Bengali</t>
-  </si>
-  <si>
     <t>बंगाली</t>
-  </si>
-  <si>
-    <t>Odia</t>
   </si>
   <si>
     <t>उड़िया</t>
   </si>
   <si>
-    <t>Assamese</t>
-  </si>
-  <si>
     <t>असमिया</t>
   </si>
   <si>
-    <t>Punjabi</t>
-  </si>
-  <si>
     <t>पंजाबी</t>
-  </si>
-  <si>
-    <t>Gujarati</t>
   </si>
   <si>
     <t>गुजराती</t>
@@ -174,12 +150,120 @@
   <si>
     <t>आपने अपना &lt;span id=\"current_badge_name\"&gt;&lt;/span&gt; भाषा समार्थक बैज जीत लिया है</t>
   </si>
+  <si>
+    <t>Konkani DV</t>
+  </si>
+  <si>
+    <t>कोंकणी डीवी</t>
+  </si>
+  <si>
+    <t>Manipuri BN</t>
+  </si>
+  <si>
+    <t>मणिपुरी बीएन</t>
+  </si>
+  <si>
+    <t>Manipuri MM</t>
+  </si>
+  <si>
+    <t>मणिपुरी एमएम</t>
+  </si>
+  <si>
+    <t>Santali OL</t>
+  </si>
+  <si>
+    <t>संथाली ओएल</t>
+  </si>
+  <si>
+    <t>Santali DV</t>
+  </si>
+  <si>
+    <t>संथाली डीवी</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>अंग्रेज़ी</t>
+  </si>
+  <si>
+    <t>ASSAMESE</t>
+  </si>
+  <si>
+    <t>BENGALI</t>
+  </si>
+  <si>
+    <t>BODO</t>
+  </si>
+  <si>
+    <t>बोडो</t>
+  </si>
+  <si>
+    <t>DOGRI</t>
+  </si>
+  <si>
+    <t>डोगरी</t>
+  </si>
+  <si>
+    <t>GUJARATI</t>
+  </si>
+  <si>
+    <t>KANNADA</t>
+  </si>
+  <si>
+    <t>KASHMIRI</t>
+  </si>
+  <si>
+    <t>कश्मीरी</t>
+  </si>
+  <si>
+    <t>MAITHILI</t>
+  </si>
+  <si>
+    <t>मैथिली</t>
+  </si>
+  <si>
+    <t>MARATHI</t>
+  </si>
+  <si>
+    <t>ODIA</t>
+  </si>
+  <si>
+    <t>NEPALI</t>
+  </si>
+  <si>
+    <t>नेपाली</t>
+  </si>
+  <si>
+    <t>PUNJABI</t>
+  </si>
+  <si>
+    <t>SANSKRIT</t>
+  </si>
+  <si>
+    <t>संस्कृत</t>
+  </si>
+  <si>
+    <t>SINDHI</t>
+  </si>
+  <si>
+    <t>सिंधी</t>
+  </si>
+  <si>
+    <t>TAMIL</t>
+  </si>
+  <si>
+    <t>URDU</t>
+  </si>
+  <si>
+    <t>उर्दू</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -222,6 +306,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -243,7 +333,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -253,6 +343,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +565,7 @@
   <dimension ref="A1:AA1002"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -947,11 +1038,11 @@
     <row r="15" spans="1:27" ht="21.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="5"/>
       <c r="B15" s="7" t="s">
-        <v>24</v>
+        <v>37</v>
       </c>
       <c r="C15" s="5"/>
       <c r="D15" s="3" t="s">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="E15" s="5"/>
       <c r="F15" s="5"/>
@@ -980,11 +1071,11 @@
     <row r="16" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="5"/>
       <c r="B16" s="7" t="s">
-        <v>2</v>
+        <v>39</v>
       </c>
       <c r="C16" s="5"/>
       <c r="D16" s="3" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="E16" s="5"/>
       <c r="F16" s="5"/>
@@ -1012,12 +1103,12 @@
     </row>
     <row r="17" spans="1:27" ht="20.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="5"/>
-      <c r="B17" s="7" t="s">
-        <v>27</v>
+      <c r="B17" s="5" t="s">
+        <v>41</v>
       </c>
       <c r="C17" s="5"/>
       <c r="D17" s="3" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="E17" s="5"/>
       <c r="F17" s="5"/>
@@ -1045,12 +1136,12 @@
     </row>
     <row r="18" spans="1:27" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="5"/>
-      <c r="B18" s="7" t="s">
-        <v>29</v>
+      <c r="B18" s="9" t="s">
+        <v>43</v>
       </c>
       <c r="C18" s="5"/>
       <c r="D18" s="3" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
       <c r="E18" s="5"/>
       <c r="F18" s="5"/>
@@ -1078,12 +1169,12 @@
     </row>
     <row r="19" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="5"/>
-      <c r="B19" s="7" t="s">
-        <v>31</v>
+      <c r="B19" s="9" t="s">
+        <v>45</v>
       </c>
       <c r="C19" s="5"/>
       <c r="D19" s="3" t="s">
-        <v>32</v>
+        <v>46</v>
       </c>
       <c r="E19" s="5"/>
       <c r="F19" s="5"/>
@@ -1111,12 +1202,12 @@
     </row>
     <row r="20" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="5"/>
-      <c r="B20" s="7" t="s">
-        <v>33</v>
+      <c r="B20" s="9" t="s">
+        <v>47</v>
       </c>
       <c r="C20" s="5"/>
       <c r="D20" s="3" t="s">
-        <v>34</v>
+        <v>48</v>
       </c>
       <c r="E20" s="5"/>
       <c r="F20" s="5"/>
@@ -1144,12 +1235,12 @@
     </row>
     <row r="21" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="5"/>
-      <c r="B21" s="7" t="s">
-        <v>35</v>
+      <c r="B21" s="9" t="s">
+        <v>49</v>
       </c>
       <c r="C21" s="5"/>
       <c r="D21" s="3" t="s">
-        <v>36</v>
+        <v>50</v>
       </c>
       <c r="E21" s="5"/>
       <c r="F21" s="5"/>
@@ -1177,12 +1268,12 @@
     </row>
     <row r="22" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="5"/>
-      <c r="B22" s="7" t="s">
-        <v>37</v>
+      <c r="B22" s="9" t="s">
+        <v>51</v>
       </c>
       <c r="C22" s="5"/>
       <c r="D22" s="3" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -1210,12 +1301,12 @@
     </row>
     <row r="23" spans="1:27" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="5"/>
-      <c r="B23" s="7" t="s">
-        <v>39</v>
+      <c r="B23" s="9" t="s">
+        <v>53</v>
       </c>
       <c r="C23" s="5"/>
       <c r="D23" s="3" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
@@ -1243,12 +1334,12 @@
     </row>
     <row r="24" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A24" s="5"/>
-      <c r="B24" s="7" t="s">
-        <v>41</v>
+      <c r="B24" s="9" t="s">
+        <v>55</v>
       </c>
       <c r="C24" s="5"/>
       <c r="D24" s="3" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
       <c r="E24" s="5"/>
       <c r="F24" s="5"/>
@@ -1276,12 +1367,12 @@
     </row>
     <row r="25" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A25" s="5"/>
-      <c r="B25" s="7" t="s">
-        <v>43</v>
+      <c r="B25" s="9" t="s">
+        <v>56</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="3" t="s">
-        <v>44</v>
+        <v>32</v>
       </c>
       <c r="E25" s="5"/>
       <c r="F25" s="5"/>
@@ -1309,12 +1400,12 @@
     </row>
     <row r="26" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A26" s="5"/>
-      <c r="B26" s="7" t="s">
-        <v>45</v>
+      <c r="B26" s="9" t="s">
+        <v>57</v>
       </c>
       <c r="C26" s="5"/>
       <c r="D26" s="3" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -1342,12 +1433,12 @@
     </row>
     <row r="27" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="5"/>
-      <c r="B27" s="7" t="s">
-        <v>47</v>
+      <c r="B27" s="9" t="s">
+        <v>59</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="3" t="s">
-        <v>48</v>
+        <v>60</v>
       </c>
       <c r="E27" s="5"/>
       <c r="F27" s="5"/>
@@ -1375,12 +1466,12 @@
     </row>
     <row r="28" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="5"/>
-      <c r="B28" s="5" t="s">
-        <v>49</v>
+      <c r="B28" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="C28" s="5"/>
       <c r="D28" s="3" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E28" s="5"/>
       <c r="F28" s="5"/>
@@ -1406,11 +1497,15 @@
       <c r="Z28" s="5"/>
       <c r="AA28" s="1"/>
     </row>
-    <row r="29" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A29" s="5"/>
-      <c r="B29" s="5"/>
+      <c r="B29" s="9" t="s">
+        <v>2</v>
+      </c>
       <c r="C29" s="5"/>
-      <c r="D29" s="5"/>
+      <c r="D29" s="3" t="s">
+        <v>26</v>
+      </c>
       <c r="E29" s="5"/>
       <c r="F29" s="5"/>
       <c r="G29" s="5"/>
@@ -1435,11 +1530,15 @@
       <c r="Z29" s="5"/>
       <c r="AA29" s="1"/>
     </row>
-    <row r="30" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" s="5"/>
-      <c r="B30" s="5"/>
+      <c r="B30" s="9" t="s">
+        <v>62</v>
+      </c>
       <c r="C30" s="5"/>
-      <c r="D30" s="5"/>
+      <c r="D30" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5"/>
@@ -1464,11 +1563,15 @@
       <c r="Z30" s="5"/>
       <c r="AA30" s="1"/>
     </row>
-    <row r="31" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="5"/>
-      <c r="B31" s="5"/>
+      <c r="B31" s="9" t="s">
+        <v>63</v>
+      </c>
       <c r="C31" s="5"/>
-      <c r="D31" s="5"/>
+      <c r="D31" s="3" t="s">
+        <v>64</v>
+      </c>
       <c r="E31" s="5"/>
       <c r="F31" s="5"/>
       <c r="G31" s="5"/>
@@ -1493,11 +1596,15 @@
       <c r="Z31" s="5"/>
       <c r="AA31" s="1"/>
     </row>
-    <row r="32" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="5"/>
-      <c r="B32" s="5"/>
+      <c r="B32" s="9" t="s">
+        <v>65</v>
+      </c>
       <c r="C32" s="5"/>
-      <c r="D32" s="5"/>
+      <c r="D32" s="3" t="s">
+        <v>66</v>
+      </c>
       <c r="E32" s="5"/>
       <c r="F32" s="5"/>
       <c r="G32" s="5"/>
@@ -1522,11 +1629,15 @@
       <c r="Z32" s="5"/>
       <c r="AA32" s="1"/>
     </row>
-    <row r="33" spans="1:27" ht="89.5" customHeight="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:27" ht="89.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="5"/>
-      <c r="B33" s="5"/>
+      <c r="B33" s="9" t="s">
+        <v>30</v>
+      </c>
       <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
+      <c r="D33" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="E33" s="5"/>
       <c r="F33" s="5"/>
       <c r="G33" s="5"/>
@@ -1551,11 +1662,15 @@
       <c r="Z33" s="5"/>
       <c r="AA33" s="1"/>
     </row>
-    <row r="34" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="34" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="5"/>
-      <c r="B34" s="5"/>
+      <c r="B34" s="9" t="s">
+        <v>67</v>
+      </c>
       <c r="C34" s="5"/>
-      <c r="D34" s="5"/>
+      <c r="D34" s="3" t="s">
+        <v>27</v>
+      </c>
       <c r="E34" s="5"/>
       <c r="F34" s="5"/>
       <c r="G34" s="5"/>
@@ -1580,11 +1695,15 @@
       <c r="Z34" s="5"/>
       <c r="AA34" s="1"/>
     </row>
-    <row r="35" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="35" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="5"/>
-      <c r="B35" s="5"/>
+      <c r="B35" s="9" t="s">
+        <v>68</v>
+      </c>
       <c r="C35" s="5"/>
-      <c r="D35" s="5"/>
+      <c r="D35" s="3" t="s">
+        <v>33</v>
+      </c>
       <c r="E35" s="5"/>
       <c r="F35" s="5"/>
       <c r="G35" s="5"/>
@@ -1609,11 +1728,15 @@
       <c r="Z35" s="5"/>
       <c r="AA35" s="1"/>
     </row>
-    <row r="36" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="36" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="5"/>
-      <c r="B36" s="5"/>
+      <c r="B36" s="9" t="s">
+        <v>69</v>
+      </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="5"/>
+      <c r="D36" s="3" t="s">
+        <v>70</v>
+      </c>
       <c r="E36" s="5"/>
       <c r="F36" s="5"/>
       <c r="G36" s="5"/>
@@ -1638,11 +1761,15 @@
       <c r="Z36" s="5"/>
       <c r="AA36" s="1"/>
     </row>
-    <row r="37" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="37" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="5"/>
-      <c r="B37" s="5"/>
+      <c r="B37" s="9" t="s">
+        <v>71</v>
+      </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="5"/>
+      <c r="D37" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="E37" s="5"/>
       <c r="F37" s="5"/>
       <c r="G37" s="5"/>
@@ -1667,11 +1794,15 @@
       <c r="Z37" s="5"/>
       <c r="AA37" s="1"/>
     </row>
-    <row r="38" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="38" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="5"/>
-      <c r="B38" s="5"/>
+      <c r="B38" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="5"/>
+      <c r="D38" s="3" t="s">
+        <v>73</v>
+      </c>
       <c r="E38" s="5"/>
       <c r="F38" s="5"/>
       <c r="G38" s="5"/>
@@ -1696,11 +1827,15 @@
       <c r="Z38" s="5"/>
       <c r="AA38" s="1"/>
     </row>
-    <row r="39" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="39" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="5"/>
-      <c r="B39" s="5"/>
+      <c r="B39" s="9" t="s">
+        <v>74</v>
+      </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="5"/>
+      <c r="D39" s="3" t="s">
+        <v>75</v>
+      </c>
       <c r="E39" s="5"/>
       <c r="F39" s="5"/>
       <c r="G39" s="5"/>
@@ -1725,11 +1860,15 @@
       <c r="Z39" s="5"/>
       <c r="AA39" s="1"/>
     </row>
-    <row r="40" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="40" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="5"/>
-      <c r="B40" s="5"/>
+      <c r="B40" s="9" t="s">
+        <v>76</v>
+      </c>
       <c r="C40" s="5"/>
-      <c r="D40" s="5"/>
+      <c r="D40" s="3" t="s">
+        <v>28</v>
+      </c>
       <c r="E40" s="5"/>
       <c r="F40" s="5"/>
       <c r="G40" s="5"/>
@@ -1754,11 +1893,15 @@
       <c r="Z40" s="5"/>
       <c r="AA40" s="1"/>
     </row>
-    <row r="41" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="41" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="5"/>
-      <c r="B41" s="5"/>
+      <c r="B41" s="9" t="s">
+        <v>24</v>
+      </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="5"/>
+      <c r="D41" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="E41" s="5"/>
       <c r="F41" s="5"/>
       <c r="G41" s="5"/>
@@ -1783,11 +1926,15 @@
       <c r="Z41" s="5"/>
       <c r="AA41" s="1"/>
     </row>
-    <row r="42" spans="1:27" ht="13" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:27" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="5"/>
-      <c r="B42" s="5"/>
+      <c r="B42" s="9" t="s">
+        <v>77</v>
+      </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="5"/>
+      <c r="D42" s="3" t="s">
+        <v>78</v>
+      </c>
       <c r="E42" s="5"/>
       <c r="F42" s="5"/>
       <c r="G42" s="5"/>

</xml_diff>